<commit_message>
removed data from excel
</commit_message>
<xml_diff>
--- a/supplier_send_list.xlsx
+++ b/supplier_send_list.xlsx
@@ -1,56 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jun\Desktop\SUPPLIER_EMAIL_TOOL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6770359C-7019-4D9D-889F-4C23F10D4D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8016" yWindow="3996" windowWidth="15048" windowHeight="8448" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SUPPLIER_LIST" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SUPPLIER_LIST" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SUPPLIER_LIST'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SUPPLIER_LIST!$A$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>SUPPLIER_NO</t>
+  </si>
+  <si>
+    <t>SENT_STATUS</t>
+  </si>
+  <si>
+    <t>SPA_EMAIL</t>
+  </si>
+  <si>
+    <t>SUPPLIER_EMAIL</t>
+  </si>
+  <si>
+    <t>ROLE_SELECTED</t>
+  </si>
+  <si>
+    <t>ROLE_FLAG</t>
+  </si>
+  <si>
+    <t>CONTACT_ERROR</t>
+  </si>
+  <si>
+    <t>FILE_ERROR</t>
+  </si>
+  <si>
+    <t>SERVER_ERROR</t>
+  </si>
+  <si>
+    <t>SERVER_RESPONSE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -83,86 +124,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -428,129 +410,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="16.109375" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="16.109375" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="29" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="21.88671875" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="41.6640625" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="13.77734375" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
-    <col width="23.88671875" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
-    <col width="14.21875" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
-    <col width="17.77734375" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
-    <col width="21.21875" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
+    <col min="1" max="1" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customHeight="1" thickBot="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>SUPPLIER_NO</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>SENT_STATUS</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>SPA_EMAIL</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>SUPPLIER_EMAIL</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>ROLE_SELECTED</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>ROLE_FLAG</t>
-        </is>
-      </c>
-      <c r="G1" s="6" t="inlineStr">
-        <is>
-          <t>CONTACT_ERROR</t>
-        </is>
-      </c>
-      <c r="H1" s="6" t="inlineStr">
-        <is>
-          <t>FILE_ERROR</t>
-        </is>
-      </c>
-      <c r="I1" s="6" t="inlineStr">
-        <is>
-          <t>SERVER_ERROR</t>
-        </is>
-      </c>
-      <c r="J1" s="6" t="inlineStr">
-        <is>
-          <t>SERVER_RESPONSE</t>
-        </is>
+    <row r="1" spans="1:10" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>20002263</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>grace.romesberg@grainger.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Dawson.parker@regalrexnord.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Primary</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>HAS_ROLE</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;&lt;soap:Envelope xmlns:soap="http://www.w3.org/2003/05/soap-envelope" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema"&gt;&lt;soap:Body&gt;&lt;SMTPEmailResponse xmlns="http://www.supplierconnect.com/LINUX_RULES"&gt;&lt;SMTPEmailResult /&gt;&lt;/SMTPEmailResponse&gt;&lt;/soap:Body&gt;&lt;/soap:Envelope&gt;</t>
-        </is>
-      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="J2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1">
-    <sortState ref="A2:J54">
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J54">
       <sortCondition descending="1" ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddHeader/>
-    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000d_# Low Sensitivity</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
+    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000D_# Low Sensitivity</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed setup to include api key and prevented repeat sf connections
</commit_message>
<xml_diff>
--- a/supplier_send_list.xlsx
+++ b/supplier_send_list.xlsx
@@ -1,97 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jun\Desktop\SUPPLIER_EMAIL_TOOL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6770359C-7019-4D9D-889F-4C23F10D4D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SUPPLIER_LIST" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SUPPLIER_LIST" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SUPPLIER_LIST!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SUPPLIER_LIST'!$A$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>SUPPLIER_NO</t>
-  </si>
-  <si>
-    <t>SENT_STATUS</t>
-  </si>
-  <si>
-    <t>SPA_EMAIL</t>
-  </si>
-  <si>
-    <t>SUPPLIER_EMAIL</t>
-  </si>
-  <si>
-    <t>ROLE_SELECTED</t>
-  </si>
-  <si>
-    <t>ROLE_FLAG</t>
-  </si>
-  <si>
-    <t>CONTACT_ERROR</t>
-  </si>
-  <si>
-    <t>FILE_ERROR</t>
-  </si>
-  <si>
-    <t>SERVER_ERROR</t>
-  </si>
-  <si>
-    <t>SERVER_RESPONSE</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,27 +83,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,8 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -419,72 +440,117 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="29" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="41.7109375" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.7109375" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
+    <col width="17.7109375" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
+    <col width="21.28515625" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
+    <row r="1" ht="16.15" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SUPPLIER_NO</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>SENT_STATUS</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>SPA_EMAIL</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>SUPPLIER_EMAIL</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>ROLE_SELECTED</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>ROLE_FLAG</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>CONTACT_ERROR</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>FILE_ERROR</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>SERVER_ERROR</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>SERVER_RESPONSE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>20002263</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="J2"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>grace.romesberg@grainger.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Dawson.parker@regalrexnord.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>HAS_ROLE</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;&lt;soap:Envelope xmlns:soap="http://www.w3.org/2003/05/soap-envelope" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema"&gt;&lt;soap:Body&gt;&lt;SMTPEmailResponse xmlns="http://www.supplierconnect.com/LINUX_RULES"&gt;&lt;SMTPEmailResult /&gt;&lt;/SMTPEmailResponse&gt;&lt;/soap:Body&gt;&lt;/soap:Envelope&gt;</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J54">
+  <autoFilter ref="A1:J1">
+    <sortState ref="A2:J54">
       <sortCondition descending="1" ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000D_# Low Sensitivity</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000d_# Low Sensitivity</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed setup user_name going in wrong folder
</commit_message>
<xml_diff>
--- a/supplier_send_list.xlsx
+++ b/supplier_send_list.xlsx
@@ -1,97 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grainger-my.sharepoint.com/personal/jeffrey_cao_grainger_ca/Documents/Desktop/supplier-email-tool/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_A8D3D462EC90A9493F04147A04E9961E2BC893EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1EB5931-1E2C-498F-A0EE-264BF67F0D3D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SUPPLIER_LIST" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SUPPLIER_LIST" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SUPPLIER_LIST!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SUPPLIER_LIST'!$A$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>SUPPLIER_NO</t>
-  </si>
-  <si>
-    <t>SENT_STATUS</t>
-  </si>
-  <si>
-    <t>SPA_EMAIL</t>
-  </si>
-  <si>
-    <t>SUPPLIER_EMAIL</t>
-  </si>
-  <si>
-    <t>ROLE_SELECTED</t>
-  </si>
-  <si>
-    <t>ROLE_FLAG</t>
-  </si>
-  <si>
-    <t>CONTACT_ERROR</t>
-  </si>
-  <si>
-    <t>FILE_ERROR</t>
-  </si>
-  <si>
-    <t>SERVER_ERROR</t>
-  </si>
-  <si>
-    <t>SERVER_RESPONSE</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,31 +87,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,81 +439,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:L2"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col width="16.109375" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="16.109375" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="29" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="58.6640625" customWidth="1" style="5" min="4" max="4"/>
+    <col width="41.6640625" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.6640625" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="23.88671875" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="14.33203125" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
+    <col width="17.6640625" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
+    <col width="21.33203125" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
+    <row r="1" ht="16.2" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SUPPLIER_NO</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>SENT_STATUS</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>SPA_EMAIL</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>SUPPLIER_EMAIL</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>ROLE_SELECTED</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>ROLE_FLAG</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>CONTACT_ERROR</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>FILE_ERROR</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>SERVER_ERROR</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>SERVER_RESPONSE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>20002263</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="J2"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>grace.romesberg@grainger.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Dawson.parker@regalrexnord.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Primary</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>HAS_ROLE</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;&lt;soap:Envelope xmlns:soap="http://www.w3.org/2003/05/soap-envelope" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema"&gt;&lt;soap:Body&gt;&lt;SMTPEmailResponse xmlns="http://www.supplierconnect.com/LINUX_RULES"&gt;&lt;SMTPEmailResult /&gt;&lt;/SMTPEmailResponse&gt;&lt;/soap:Body&gt;&lt;/soap:Envelope&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>20001554</v>
+      </c>
+      <c r="D3" s="7" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J54">
+  <autoFilter ref="A1:J1">
+    <sortState ref="A2:J54">
       <sortCondition descending="1" ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000D_# Low Sensitivity</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000d_# Low Sensitivity</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed spacing issue in file read in SMTP_backend
</commit_message>
<xml_diff>
--- a/supplier_send_list.xlsx
+++ b/supplier_send_list.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SUPPLIER_LIST" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SUPPLIER_LIST" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SUPPLIER_LIST'!$A$1:$J$1</definedName>

</xml_diff>